<commit_message>
added excel to node route controller
</commit_message>
<xml_diff>
--- a/uploads/Employee.xlsx
+++ b/uploads/Employee.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>S no</t>
   </si>
@@ -34,58 +34,49 @@
     <t>Employee Bio</t>
   </si>
   <si>
-    <t>john</t>
-  </si>
-  <si>
-    <t>10 avenue</t>
-  </si>
-  <si>
-    <t>johns@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">back-end </t>
-  </si>
-  <si>
-    <t>mike</t>
-  </si>
-  <si>
-    <t>mike@gmail.com</t>
+    <t>john doe</t>
+  </si>
+  <si>
+    <t>10 clover lane</t>
+  </si>
+  <si>
+    <t>john@gmail.com</t>
   </si>
   <si>
     <t>ux designer</t>
   </si>
   <si>
-    <t>mike doe</t>
-  </si>
-  <si>
-    <t>10 frontlane avenue</t>
-  </si>
-  <si>
-    <t>mikee@gmail.com</t>
-  </si>
-  <si>
-    <t>ui developer</t>
-  </si>
-  <si>
-    <t>johndoes</t>
-  </si>
-  <si>
-    <t>johndore@gmail.com</t>
-  </si>
-  <si>
-    <t>doe@gmail.com</t>
-  </si>
-  <si>
-    <t>bio here</t>
-  </si>
-  <si>
-    <t>johndos</t>
-  </si>
-  <si>
-    <t>doe@gmil.com</t>
-  </si>
-  <si>
-    <t>bio herr</t>
+    <t>tracy</t>
+  </si>
+  <si>
+    <t>10 field lane</t>
+  </si>
+  <si>
+    <t>tracy@gmail.com</t>
+  </si>
+  <si>
+    <t>java developer</t>
+  </si>
+  <si>
+    <t>oliver queen</t>
+  </si>
+  <si>
+    <t>starline city</t>
+  </si>
+  <si>
+    <t>oliver@gmail.com</t>
+  </si>
+  <si>
+    <t>a full stack developer</t>
+  </si>
+  <si>
+    <t>bhavesh</t>
+  </si>
+  <si>
+    <t>10 front lane</t>
+  </si>
+  <si>
+    <t>bhavesh@gmai.com</t>
   </si>
 </sst>
 </file>
@@ -467,7 +458,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="7" width="10" customWidth="1"/>
@@ -510,10 +501,10 @@
         <v>9</v>
       </c>
       <c r="E2" s="2">
-        <v>44138</v>
+        <v>43839</v>
       </c>
       <c r="F2">
-        <v>745421</v>
+        <v>784521</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -527,19 +518,19 @@
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>43112</v>
+        <v>44143</v>
       </c>
       <c r="F3">
-        <v>78451</v>
+        <v>54875421</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -547,22 +538,22 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E4" s="2">
-        <v>44140</v>
+        <v>44134</v>
       </c>
       <c r="F4">
-        <v>785421</v>
+        <v>78545212</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -570,45 +561,22 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E5" s="2">
-        <v>44147</v>
+        <v>44140</v>
       </c>
       <c r="F5">
-        <v>87542154785421</v>
+        <v>784512</v>
       </c>
       <c r="G5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="2">
-        <v>44146</v>
-      </c>
-      <c r="F6">
-        <v>8754215</v>
-      </c>
-      <c r="G6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>